<commit_message>
variable traceability from script to spreadsheet
</commit_message>
<xml_diff>
--- a/Population/data/Population Indicators.xlsx
+++ b/Population/data/Population Indicators.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\JusticeCOVID\Population\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFC4215-1F46-4688-B593-FA837E30F2B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA10BBBC-39B9-4855-9738-4071DA6F421D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B9AFA079-0671-40AD-860D-809D829A87F1}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B9AFA079-0671-40AD-860D-809D829A87F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Summaries" sheetId="1" r:id="rId1"/>
-    <sheet name="AU Pop" sheetId="2" r:id="rId2"/>
-    <sheet name="A&amp;TSI Pop" sheetId="7" r:id="rId3"/>
-    <sheet name="Prison Pop" sheetId="3" r:id="rId4"/>
-    <sheet name="Prison Chronic Conditions" sheetId="4" r:id="rId5"/>
-    <sheet name="Obesity" sheetId="8" r:id="rId6"/>
-    <sheet name="COPD" sheetId="9" r:id="rId7"/>
-    <sheet name="Hypertension" sheetId="10" r:id="rId8"/>
+    <sheet name="Data Traceability" sheetId="11" r:id="rId2"/>
+    <sheet name="AU Pop" sheetId="2" r:id="rId3"/>
+    <sheet name="A&amp;TSI Pop" sheetId="7" r:id="rId4"/>
+    <sheet name="Prison Pop" sheetId="3" r:id="rId5"/>
+    <sheet name="Prison Chronic Conditions" sheetId="4" r:id="rId6"/>
+    <sheet name="Obesity" sheetId="8" r:id="rId7"/>
+    <sheet name="COPD" sheetId="9" r:id="rId8"/>
+    <sheet name="Hypertension" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1794,7 +1795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="687">
   <si>
     <t>&lt; 10</t>
   </si>
@@ -3767,12 +3768,231 @@
   <si>
     <t>AU Deaths 27/5/2020</t>
   </si>
+  <si>
+    <t>Overweight</t>
+  </si>
+  <si>
+    <t>prisoner_health.html</t>
+  </si>
+  <si>
+    <t>prisoner_population.html</t>
+  </si>
+  <si>
+    <t>age1</t>
+  </si>
+  <si>
+    <t>age2</t>
+  </si>
+  <si>
+    <t>0-9</t>
+  </si>
+  <si>
+    <t>covid19_prisoner_impact.html</t>
+  </si>
+  <si>
+    <t>chronic_illnesses</t>
+  </si>
+  <si>
+    <t>au_population_chronic_illness</t>
+  </si>
+  <si>
+    <t>male_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>female_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>age_18_24_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>age_25_34_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>age_35_44_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>age_45_54_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>age_55plus_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>age_full</t>
+  </si>
+  <si>
+    <t>total_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>male_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>female_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>nonIndigenous_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>Indigenous_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>male_nonIndigenous_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>female_nonIndigenous_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>male_Indigenous_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>female_Indigenous_per1k_prisoners</t>
+  </si>
+  <si>
+    <t>nonIndigenous_total_prisoners</t>
+  </si>
+  <si>
+    <t>Indigenous_total_prisoners</t>
+  </si>
+  <si>
+    <t>male_adult_nonIndigenous_prisoners</t>
+  </si>
+  <si>
+    <t>female_adult_nonIndigenous_prisoners</t>
+  </si>
+  <si>
+    <t>male_adult_Indigenous_prisoners</t>
+  </si>
+  <si>
+    <t>female_adult_Indigenous_prisoners</t>
+  </si>
+  <si>
+    <t>total_adult_prisoners</t>
+  </si>
+  <si>
+    <t>male_nonIndigenous_population_perc</t>
+  </si>
+  <si>
+    <t>female_nonIndigenous_population_perc</t>
+  </si>
+  <si>
+    <t>male_Indigenous_population_perc</t>
+  </si>
+  <si>
+    <t>female_Indigenous_population_perc</t>
+  </si>
+  <si>
+    <t>male_nonIndigenous_population_all</t>
+  </si>
+  <si>
+    <t>female_nonIndigenous_population_all</t>
+  </si>
+  <si>
+    <t>male_Indigenous_population_all</t>
+  </si>
+  <si>
+    <t>female_Indigenous_population_all</t>
+  </si>
+  <si>
+    <t>male_prisoners</t>
+  </si>
+  <si>
+    <t>female_prisoners</t>
+  </si>
+  <si>
+    <t>non_indigenous_per1K_count</t>
+  </si>
+  <si>
+    <t>indigenous_per1K_count</t>
+  </si>
+  <si>
+    <t>indigenous_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>non_indigenous_prisoner_chronic_illness</t>
+  </si>
+  <si>
+    <t>prisoner_count_by_age1</t>
+  </si>
+  <si>
+    <t>au_covid19_mortality_by_age1</t>
+  </si>
+  <si>
+    <t>cn_covid19_mortality_by_age1</t>
+  </si>
+  <si>
+    <t>it_covid19_mortality_by_age1</t>
+  </si>
+  <si>
+    <t>kr_covid19_mortality_by_age1</t>
+  </si>
+  <si>
+    <t>es_covid19_mortality_by_age1</t>
+  </si>
+  <si>
+    <t>covid19_mortality_by_chronic_illness</t>
+  </si>
+  <si>
+    <t>male_staff</t>
+  </si>
+  <si>
+    <t>female_staff</t>
+  </si>
+  <si>
+    <t>indigenous_prisoners</t>
+  </si>
+  <si>
+    <t>indigenous_population</t>
+  </si>
+  <si>
+    <t>non_indigenous_prisoners</t>
+  </si>
+  <si>
+    <t>non_indigenous_population</t>
+  </si>
+  <si>
+    <t>au_sex_covid19_mortality</t>
+  </si>
+  <si>
+    <t>cn_sex_covid19_mortality</t>
+  </si>
+  <si>
+    <t>it_sex_covid19_mortality</t>
+  </si>
+  <si>
+    <t>kr_sex_covid19_mortality</t>
+  </si>
+  <si>
+    <t>es_sex_covid19_mortality</t>
+  </si>
+  <si>
+    <t>au_covid19_mortality_by_age2</t>
+  </si>
+  <si>
+    <t>cn_covid19_mortality_by_age2</t>
+  </si>
+  <si>
+    <t>it_covid19_mortality_by_age2</t>
+  </si>
+  <si>
+    <t>kr_covid19_mortality_by_age2</t>
+  </si>
+  <si>
+    <t>es_covid19_mortality_by_age2</t>
+  </si>
+  <si>
+    <t>prisoner_count_by_age2</t>
+  </si>
+  <si>
+    <t>non_indigenous_prisoner_count_by_age2</t>
+  </si>
+  <si>
+    <t>indigenous_prisoner_count_by_age2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -3780,6 +4000,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;&quot;#,##0.0&quot;&quot;"/>
     <numFmt numFmtId="168" formatCode="&quot;#&quot;#,##0.0"/>
+    <numFmt numFmtId="173" formatCode="0.000"/>
   </numFmts>
   <fonts count="64">
     <font>
@@ -4215,7 +4436,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4428,6 +4649,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5204,7 +5431,7 @@
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="432">
+  <cellXfs count="441">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -5871,11 +6098,11 @@
     <xf numFmtId="3" fontId="38" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="38" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="38" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5886,50 +6113,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="38" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="38" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5946,6 +6137,42 @@
     <xf numFmtId="3" fontId="38" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5961,24 +6188,6 @@
     <xf numFmtId="0" fontId="32" fillId="33" borderId="24" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="35" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="42" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5990,6 +6199,24 @@
     </xf>
     <xf numFmtId="49" fontId="42" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="35" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="59" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -6008,6 +6235,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="24" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6017,12 +6250,15 @@
     <xf numFmtId="49" fontId="42" fillId="37" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="73">
     <cellStyle name="20% - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -6422,8 +6658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69445D4F-6ED8-41C8-8CD1-A1D8E95413A8}">
   <dimension ref="A2:AJ160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="J105" sqref="J105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7415,17 +7651,17 @@
       <c r="A43" s="295" t="s">
         <v>526</v>
       </c>
-      <c r="B43" s="388" t="s">
+      <c r="B43" s="402" t="s">
         <v>432</v>
       </c>
-      <c r="C43" s="389"/>
-      <c r="D43" s="389"/>
-      <c r="E43" s="389"/>
-      <c r="F43" s="389"/>
-      <c r="G43" s="389"/>
-      <c r="H43" s="389"/>
-      <c r="I43" s="389"/>
-      <c r="J43" s="390"/>
+      <c r="C43" s="403"/>
+      <c r="D43" s="403"/>
+      <c r="E43" s="403"/>
+      <c r="F43" s="403"/>
+      <c r="G43" s="403"/>
+      <c r="H43" s="403"/>
+      <c r="I43" s="403"/>
+      <c r="J43" s="404"/>
       <c r="K43" s="382" t="s">
         <v>237</v>
       </c>
@@ -7437,64 +7673,64 @@
       <c r="Q43" s="383"/>
       <c r="R43" s="383"/>
       <c r="S43" s="384"/>
-      <c r="T43" s="387" t="s">
+      <c r="T43" s="385" t="s">
         <v>523</v>
       </c>
-      <c r="U43" s="387"/>
-      <c r="V43" s="387"/>
-      <c r="W43" s="387"/>
-      <c r="X43" s="387"/>
-      <c r="Y43" s="387"/>
-      <c r="Z43" s="387"/>
-      <c r="AA43" s="387"/>
-      <c r="AB43" s="387"/>
+      <c r="U43" s="385"/>
+      <c r="V43" s="385"/>
+      <c r="W43" s="385"/>
+      <c r="X43" s="385"/>
+      <c r="Y43" s="385"/>
+      <c r="Z43" s="385"/>
+      <c r="AA43" s="385"/>
+      <c r="AB43" s="385"/>
     </row>
     <row r="44" spans="1:28" ht="15" customHeight="1">
-      <c r="B44" s="387" t="s">
+      <c r="B44" s="385" t="s">
         <v>180</v>
       </c>
-      <c r="C44" s="387"/>
-      <c r="D44" s="387"/>
-      <c r="E44" s="387" t="s">
+      <c r="C44" s="385"/>
+      <c r="D44" s="385"/>
+      <c r="E44" s="385" t="s">
         <v>181</v>
       </c>
-      <c r="F44" s="387"/>
-      <c r="G44" s="387"/>
-      <c r="H44" s="387" t="s">
+      <c r="F44" s="385"/>
+      <c r="G44" s="385"/>
+      <c r="H44" s="385" t="s">
         <v>433</v>
       </c>
-      <c r="I44" s="387"/>
-      <c r="J44" s="387"/>
-      <c r="K44" s="397" t="s">
+      <c r="I44" s="385"/>
+      <c r="J44" s="385"/>
+      <c r="K44" s="393" t="s">
         <v>180</v>
       </c>
-      <c r="L44" s="397"/>
-      <c r="M44" s="397"/>
-      <c r="N44" s="397" t="s">
+      <c r="L44" s="393"/>
+      <c r="M44" s="393"/>
+      <c r="N44" s="393" t="s">
         <v>181</v>
       </c>
-      <c r="O44" s="397"/>
-      <c r="P44" s="397"/>
+      <c r="O44" s="393"/>
+      <c r="P44" s="393"/>
       <c r="Q44" s="382" t="s">
         <v>433</v>
       </c>
       <c r="R44" s="383"/>
       <c r="S44" s="384"/>
-      <c r="T44" s="387" t="s">
+      <c r="T44" s="385" t="s">
         <v>180</v>
       </c>
-      <c r="U44" s="387"/>
-      <c r="V44" s="387"/>
-      <c r="W44" s="387" t="s">
+      <c r="U44" s="385"/>
+      <c r="V44" s="385"/>
+      <c r="W44" s="385" t="s">
         <v>181</v>
       </c>
-      <c r="X44" s="387"/>
-      <c r="Y44" s="387"/>
-      <c r="Z44" s="387" t="s">
+      <c r="X44" s="385"/>
+      <c r="Y44" s="385"/>
+      <c r="Z44" s="385" t="s">
         <v>433</v>
       </c>
-      <c r="AA44" s="387"/>
-      <c r="AB44" s="387"/>
+      <c r="AA44" s="385"/>
+      <c r="AB44" s="385"/>
     </row>
     <row r="45" spans="1:28">
       <c r="B45" s="66" t="s">
@@ -8474,10 +8710,10 @@
       <c r="A58" s="295" t="s">
         <v>527</v>
       </c>
-      <c r="B58" s="387">
+      <c r="B58" s="385">
         <v>2019</v>
       </c>
-      <c r="C58" s="387"/>
+      <c r="C58" s="385"/>
       <c r="D58" s="382">
         <v>2016</v>
       </c>
@@ -8511,8 +8747,8 @@
       <c r="Z58" s="384">
         <v>2016</v>
       </c>
-      <c r="AA58" s="387"/>
-      <c r="AB58" s="387"/>
+      <c r="AA58" s="385"/>
+      <c r="AB58" s="385"/>
       <c r="AC58" s="382">
         <v>2019</v>
       </c>
@@ -8757,8 +8993,8 @@
       <c r="AG61" s="74"/>
       <c r="AH61" s="74"/>
       <c r="AI61" s="26">
-        <f>SUM(I64:I68,K64:K68,M64:M68)</f>
-        <v>61540</v>
+        <f>SUM(M64:M68)</f>
+        <v>30770</v>
       </c>
       <c r="AJ61" t="s">
         <v>263</v>
@@ -8776,19 +9012,19 @@
         <f>'AU Pop'!H22</f>
         <v>9.5612474089386751E-2</v>
       </c>
-      <c r="D62" s="403">
+      <c r="D62" s="391">
         <f>'A&amp;TSI Pop'!L11</f>
         <v>1405253</v>
       </c>
-      <c r="E62" s="380">
+      <c r="E62" s="396">
         <f t="shared" ref="E62:E68" si="12">D62/SUM($D$61:$D$68)</f>
         <v>0.12109420846479671</v>
       </c>
-      <c r="F62" s="385">
+      <c r="F62" s="386">
         <f>'A&amp;TSI Pop'!L29</f>
         <v>1333829</v>
       </c>
-      <c r="G62" s="380">
+      <c r="G62" s="396">
         <f t="shared" ref="G62:G70" si="13">F62/SUM($F$61:$F$68)</f>
         <v>0.11315223148858543</v>
       </c>
@@ -8800,23 +9036,23 @@
       <c r="K62" s="58"/>
       <c r="M62" s="58"/>
       <c r="N62" s="74"/>
-      <c r="O62" s="391">
+      <c r="O62" s="394">
         <f>'A&amp;TSI Pop'!H11</f>
         <v>85770</v>
       </c>
-      <c r="P62" s="380">
+      <c r="P62" s="396">
         <f t="shared" ref="P62:P70" si="14">O62/SUM($O$61:$O$68)</f>
         <v>0.21527911990823592</v>
       </c>
-      <c r="Q62" s="393">
+      <c r="Q62" s="398">
         <f>'A&amp;TSI Pop'!H29</f>
         <v>81992</v>
       </c>
-      <c r="R62" s="380">
+      <c r="R62" s="396">
         <f t="shared" ref="R62:R70" si="15">Q62/SUM($Q$61:$Q$68)</f>
         <v>0.20500460055206624</v>
       </c>
-      <c r="S62" s="395">
+      <c r="S62" s="400">
         <f>'A&amp;TSI Pop'!H47</f>
         <v>167762</v>
       </c>
@@ -8824,15 +9060,15 @@
       <c r="V62" s="58"/>
       <c r="X62" s="74"/>
       <c r="Y62" s="74"/>
-      <c r="Z62" s="385">
+      <c r="Z62" s="386">
         <f>O62+D62</f>
         <v>1491023</v>
       </c>
-      <c r="AA62" s="400">
+      <c r="AA62" s="388">
         <f>Q62+F62</f>
         <v>1415821</v>
       </c>
-      <c r="AB62" s="402">
+      <c r="AB62" s="390">
         <f>S62+H62</f>
         <v>2906844</v>
       </c>
@@ -8856,10 +9092,10 @@
         <f>'AU Pop'!H25</f>
         <v>2.4952286703894818E-2</v>
       </c>
-      <c r="D63" s="404"/>
-      <c r="E63" s="381"/>
-      <c r="F63" s="386"/>
-      <c r="G63" s="381"/>
+      <c r="D63" s="392"/>
+      <c r="E63" s="397"/>
+      <c r="F63" s="387"/>
+      <c r="G63" s="397"/>
       <c r="H63" s="364"/>
       <c r="I63" s="80">
         <f>'Prison Pop'!L58</f>
@@ -8874,11 +9110,11 @@
         <v>376</v>
       </c>
       <c r="N63" s="74"/>
-      <c r="O63" s="392"/>
-      <c r="P63" s="381"/>
-      <c r="Q63" s="394"/>
-      <c r="R63" s="381"/>
-      <c r="S63" s="396"/>
+      <c r="O63" s="395"/>
+      <c r="P63" s="397"/>
+      <c r="Q63" s="399"/>
+      <c r="R63" s="397"/>
+      <c r="S63" s="401"/>
       <c r="T63" s="80">
         <f>'Prison Pop'!L6</f>
         <v>348</v>
@@ -8892,9 +9128,9 @@
         <v>378</v>
       </c>
       <c r="Y63" s="74"/>
-      <c r="Z63" s="386"/>
-      <c r="AA63" s="401"/>
-      <c r="AB63" s="401"/>
+      <c r="Z63" s="387"/>
+      <c r="AA63" s="389"/>
+      <c r="AB63" s="389"/>
       <c r="AC63" s="80">
         <f t="shared" ref="AC63:AC68" si="18">T63+I63</f>
         <v>701</v>
@@ -8910,7 +9146,7 @@
       <c r="AH63" s="74"/>
       <c r="AI63" s="214">
         <f>AI61/(AI59/1000)</f>
-        <v>3.4767888188641045</v>
+        <v>1.7383944094320523</v>
       </c>
     </row>
     <row r="64" spans="1:36">
@@ -9608,8 +9844,8 @@
         <v>0.40987377896792981</v>
       </c>
       <c r="AI68" s="26">
-        <f>SUM(T64:T68,V64:V68,X64:X68)</f>
-        <v>22994</v>
+        <f>SUM(X64:X68)</f>
+        <v>11497</v>
       </c>
       <c r="AJ68" t="s">
         <v>263</v>
@@ -9773,17 +10009,17 @@
       <c r="AH70" s="216"/>
       <c r="AI70" s="214">
         <f>AI68/(AI66/1000)</f>
-        <v>51.915153020331211</v>
+        <v>25.957576510165605</v>
       </c>
     </row>
     <row r="72" spans="1:36">
       <c r="A72" s="295" t="s">
         <v>528</v>
       </c>
-      <c r="B72" s="387">
+      <c r="B72" s="385">
         <v>2019</v>
       </c>
-      <c r="C72" s="387"/>
+      <c r="C72" s="385"/>
       <c r="D72" s="382">
         <v>2016</v>
       </c>
@@ -9814,11 +10050,11 @@
       <c r="W72" s="383"/>
       <c r="X72" s="383"/>
       <c r="Y72" s="384"/>
-      <c r="Z72" s="387">
+      <c r="Z72" s="385">
         <v>2016</v>
       </c>
-      <c r="AA72" s="387"/>
-      <c r="AB72" s="387"/>
+      <c r="AA72" s="385"/>
+      <c r="AB72" s="385"/>
       <c r="AC72" s="382">
         <v>2019</v>
       </c>
@@ -11253,18 +11489,18 @@
     <row r="103" spans="1:12">
       <c r="A103" s="1"/>
       <c r="B103" s="197"/>
-      <c r="C103" s="398" t="s">
+      <c r="C103" s="380" t="s">
         <v>11</v>
       </c>
-      <c r="D103" s="399"/>
-      <c r="E103" s="398" t="s">
+      <c r="D103" s="381"/>
+      <c r="E103" s="380" t="s">
         <v>237</v>
       </c>
-      <c r="F103" s="399"/>
-      <c r="G103" s="398" t="s">
+      <c r="F103" s="381"/>
+      <c r="G103" s="380" t="s">
         <v>146</v>
       </c>
-      <c r="H103" s="399"/>
+      <c r="H103" s="381"/>
       <c r="I103" s="197"/>
       <c r="J103" s="197"/>
     </row>
@@ -11889,15 +12125,15 @@
         <v>78.018749999999997</v>
       </c>
       <c r="I118" s="357">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="J118" s="202">
         <f t="shared" si="44"/>
-        <v>534.375</v>
+        <v>546.25</v>
       </c>
       <c r="K118" s="203">
         <f t="shared" si="45"/>
-        <v>33.665624999999999</v>
+        <v>34.41375</v>
       </c>
       <c r="L118" s="299">
         <v>0.11</v>
@@ -11934,11 +12170,11 @@
       </c>
       <c r="U118" s="167">
         <f t="shared" si="48"/>
-        <v>7623.75</v>
+        <v>7635.625</v>
       </c>
       <c r="V118" s="203">
         <f t="shared" si="49"/>
-        <v>420.79062499999998</v>
+        <v>421.53874999999999</v>
       </c>
       <c r="X118" s="197"/>
       <c r="Y118" s="110">
@@ -11994,15 +12230,15 @@
         <v>90.946319999999986</v>
       </c>
       <c r="I119" s="358">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="J119" s="181">
         <f t="shared" si="44"/>
-        <v>1401.57</v>
+        <v>1432.7159999999999</v>
       </c>
       <c r="K119" s="190">
         <f t="shared" si="45"/>
-        <v>88.298909999999992</v>
+        <v>90.261107999999993</v>
       </c>
       <c r="L119" s="298">
         <v>0.19</v>
@@ -12039,11 +12275,11 @@
       </c>
       <c r="U119" s="103">
         <f t="shared" si="48"/>
-        <v>20307.191999999999</v>
+        <v>20338.338</v>
       </c>
       <c r="V119" s="189">
         <f t="shared" si="49"/>
-        <v>924.56901000000005</v>
+        <v>926.53120800000011</v>
       </c>
       <c r="X119" s="197"/>
       <c r="Y119" s="111">
@@ -12823,6 +13059,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="D58:H58"/>
+    <mergeCell ref="D59:H59"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="T43:AB43"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="K43:S43"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="T44:V44"/>
+    <mergeCell ref="T72:Y72"/>
+    <mergeCell ref="T73:Y73"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="Z44:AB44"/>
+    <mergeCell ref="O62:O63"/>
+    <mergeCell ref="P62:P63"/>
+    <mergeCell ref="R62:R63"/>
+    <mergeCell ref="Q62:Q63"/>
+    <mergeCell ref="S62:S63"/>
+    <mergeCell ref="O58:S58"/>
+    <mergeCell ref="O59:S59"/>
+    <mergeCell ref="O72:S72"/>
+    <mergeCell ref="O73:S73"/>
+    <mergeCell ref="T58:Y58"/>
+    <mergeCell ref="T59:Y59"/>
+    <mergeCell ref="I72:N72"/>
+    <mergeCell ref="I73:N73"/>
+    <mergeCell ref="D72:H72"/>
+    <mergeCell ref="D73:H73"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="I58:N58"/>
+    <mergeCell ref="I59:N59"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="N44:P44"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="E103:F103"/>
     <mergeCell ref="G103:H103"/>
@@ -12839,48 +13117,6 @@
     <mergeCell ref="Z73:AB73"/>
     <mergeCell ref="B83:J83"/>
     <mergeCell ref="D62:D63"/>
-    <mergeCell ref="I59:N59"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="I58:N58"/>
-    <mergeCell ref="I72:N72"/>
-    <mergeCell ref="I73:N73"/>
-    <mergeCell ref="D72:H72"/>
-    <mergeCell ref="D73:H73"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="T72:Y72"/>
-    <mergeCell ref="T73:Y73"/>
-    <mergeCell ref="W44:Y44"/>
-    <mergeCell ref="Z44:AB44"/>
-    <mergeCell ref="O62:O63"/>
-    <mergeCell ref="P62:P63"/>
-    <mergeCell ref="R62:R63"/>
-    <mergeCell ref="Q62:Q63"/>
-    <mergeCell ref="S62:S63"/>
-    <mergeCell ref="O58:S58"/>
-    <mergeCell ref="O59:S59"/>
-    <mergeCell ref="O72:S72"/>
-    <mergeCell ref="O73:S73"/>
-    <mergeCell ref="T58:Y58"/>
-    <mergeCell ref="T59:Y59"/>
-    <mergeCell ref="T43:AB43"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="B43:J43"/>
-    <mergeCell ref="K43:S43"/>
-    <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="T44:V44"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="D58:H58"/>
-    <mergeCell ref="D59:H59"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31" r:id="rId1" location="case-fatality-rate-of-covid-19-by-preexisting-health-conditions" xr:uid="{7F3EF4B5-28AC-495F-9AED-D8A19838DCA0}"/>
@@ -12914,6 +13150,2276 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A3361E-C79A-4ECF-AC8C-A789F3D7C0DB}">
+  <dimension ref="A1:I98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L85" sqref="L85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="302" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>621</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>525</v>
+      </c>
+      <c r="E2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>622</v>
+      </c>
+      <c r="B3">
+        <f>'Data Summaries'!B32</f>
+        <v>0.05</v>
+      </c>
+      <c r="C3">
+        <f>'Data Summaries'!B33</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D3" s="437">
+        <f>COPD!G14</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E3">
+        <f>'Data Summaries'!B35</f>
+        <v>0.112</v>
+      </c>
+      <c r="F3" s="439">
+        <f>Hypertension!B4/100</f>
+        <v>0.33665999999999996</v>
+      </c>
+      <c r="G3">
+        <f>'Data Summaries'!B37</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H3">
+        <f>'Data Summaries'!B38</f>
+        <v>0.152</v>
+      </c>
+      <c r="I3" s="437">
+        <f>'Data Summaries'!AB55</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>623</v>
+      </c>
+      <c r="B4" s="432">
+        <f>'Data Summaries'!C116</f>
+        <v>0.04</v>
+      </c>
+      <c r="C4" s="432">
+        <f>'Data Summaries'!F116</f>
+        <v>0.06</v>
+      </c>
+      <c r="D4" s="433">
+        <f>'Data Summaries'!I116</f>
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E4" s="432">
+        <f>'Data Summaries'!L116</f>
+        <v>0.13</v>
+      </c>
+      <c r="F4" s="432">
+        <f>'Data Summaries'!O116</f>
+        <v>0.36</v>
+      </c>
+      <c r="G4" s="432">
+        <f>'Data Summaries'!R116</f>
+        <v>0.01</v>
+      </c>
+      <c r="H4" s="432">
+        <f>'Data Summaries'!AA116</f>
+        <v>0.74</v>
+      </c>
+      <c r="I4" s="439">
+        <f>'Data Summaries'!V55</f>
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>624</v>
+      </c>
+      <c r="B5" s="432">
+        <f>'Data Summaries'!C117</f>
+        <v>0.03</v>
+      </c>
+      <c r="C5" s="432">
+        <f>'Data Summaries'!F117</f>
+        <v>0.03</v>
+      </c>
+      <c r="D5" s="433">
+        <f>'Data Summaries'!I117</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E5" s="432">
+        <f>'Data Summaries'!L117</f>
+        <v>0.27</v>
+      </c>
+      <c r="F5" s="433">
+        <f>'Data Summaries'!O117</f>
+        <v>0.314</v>
+      </c>
+      <c r="G5" s="432">
+        <f>'Data Summaries'!R117</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="432">
+        <f>'Data Summaries'!AA117</f>
+        <v>0.86</v>
+      </c>
+      <c r="I5" s="439">
+        <f>'Data Summaries'!Y55</f>
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>659</v>
+      </c>
+      <c r="B6" s="432">
+        <f>'Data Summaries'!C118</f>
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="432">
+        <f>'Data Summaries'!F118</f>
+        <v>0.09</v>
+      </c>
+      <c r="D6" s="439">
+        <f>'Data Summaries'!I118</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E6" s="432">
+        <f>'Data Summaries'!L118</f>
+        <v>0.11</v>
+      </c>
+      <c r="F6" s="439">
+        <f>'Data Summaries'!O118</f>
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G6" s="432">
+        <f>'Data Summaries'!R118</f>
+        <v>0.01</v>
+      </c>
+      <c r="H6" s="432">
+        <f>'Data Summaries'!AA118</f>
+        <v>0.8</v>
+      </c>
+      <c r="I6" s="439">
+        <f>'Data Summaries'!J55</f>
+        <v>0.72400000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>660</v>
+      </c>
+      <c r="B7" s="432">
+        <f>'Data Summaries'!C119</f>
+        <v>0.03</v>
+      </c>
+      <c r="C7" s="432">
+        <f>'Data Summaries'!F119</f>
+        <v>0.04</v>
+      </c>
+      <c r="D7" s="439">
+        <f>'Data Summaries'!I119</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E7" s="432">
+        <f>'Data Summaries'!L119</f>
+        <v>0.19</v>
+      </c>
+      <c r="F7" s="439">
+        <f>'Data Summaries'!O119</f>
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G7" s="432">
+        <f>'Data Summaries'!R119</f>
+        <v>0.01</v>
+      </c>
+      <c r="H7" s="432">
+        <f>'Data Summaries'!AA119</f>
+        <v>0.73</v>
+      </c>
+      <c r="I7" s="439">
+        <f>'Data Summaries'!S55</f>
+        <v>0.626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="301" customFormat="1">
+      <c r="A8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" s="432"/>
+      <c r="H8" s="432"/>
+      <c r="I8" s="436"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>625</v>
+      </c>
+      <c r="B9" s="432">
+        <f>'Data Summaries'!C120</f>
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="432">
+        <f>'Data Summaries'!F120</f>
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="434">
+        <f>'Data Summaries'!I120</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="432">
+        <f>'Data Summaries'!L120</f>
+        <v>0.18</v>
+      </c>
+      <c r="F9" s="434">
+        <f>'Data Summaries'!O120</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G9" s="432">
+        <f>'Data Summaries'!R120</f>
+        <v>0.01</v>
+      </c>
+      <c r="H9" s="432">
+        <f>'Data Summaries'!AA120</f>
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="439">
+        <f>'Data Summaries'!AB46</f>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>626</v>
+      </c>
+      <c r="B10" s="432">
+        <f>'Data Summaries'!C121</f>
+        <v>0.02</v>
+      </c>
+      <c r="C10" s="432">
+        <f>'Data Summaries'!F121</f>
+        <v>0.03</v>
+      </c>
+      <c r="D10" s="434">
+        <f>'Data Summaries'!I121</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="432">
+        <f>'Data Summaries'!L121</f>
+        <v>0.15</v>
+      </c>
+      <c r="F10" s="434">
+        <f>'Data Summaries'!O121</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G10" s="432">
+        <f>'Data Summaries'!R121</f>
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="432">
+        <f>'Data Summaries'!AA121</f>
+        <v>0.76</v>
+      </c>
+      <c r="I10" s="439">
+        <f>'Data Summaries'!AB47</f>
+        <v>0.57700000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>627</v>
+      </c>
+      <c r="B11" s="432">
+        <f>'Data Summaries'!C122</f>
+        <v>0.04</v>
+      </c>
+      <c r="C11" s="432">
+        <f>'Data Summaries'!F122</f>
+        <v>0.08</v>
+      </c>
+      <c r="D11" s="434">
+        <f>'Data Summaries'!I122</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="432">
+        <f>'Data Summaries'!L122</f>
+        <v>0.15</v>
+      </c>
+      <c r="F11" s="434">
+        <f>'Data Summaries'!O122</f>
+        <v>0.159</v>
+      </c>
+      <c r="G11" s="432">
+        <f>'Data Summaries'!R122</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="432">
+        <f>'Data Summaries'!AA122</f>
+        <v>0.79</v>
+      </c>
+      <c r="I11" s="439">
+        <f>'Data Summaries'!AB48</f>
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>628</v>
+      </c>
+      <c r="B12" s="432">
+        <f>'Data Summaries'!C123</f>
+        <v>0.04</v>
+      </c>
+      <c r="C12" s="432">
+        <f>'Data Summaries'!F123</f>
+        <v>0.08</v>
+      </c>
+      <c r="D12" s="434">
+        <f>'Data Summaries'!I123</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E12" s="432">
+        <f>'Data Summaries'!L123</f>
+        <v>0.18</v>
+      </c>
+      <c r="F12" s="434">
+        <f>'Data Summaries'!O123</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="G12" s="432">
+        <f>'Data Summaries'!R123</f>
+        <v>0.03</v>
+      </c>
+      <c r="H12" s="432">
+        <f>'Data Summaries'!AA123</f>
+        <v>0.66</v>
+      </c>
+      <c r="I12" s="439">
+        <f>'Data Summaries'!AB49</f>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>629</v>
+      </c>
+      <c r="B13" s="432">
+        <f>'Data Summaries'!C124</f>
+        <v>0.38</v>
+      </c>
+      <c r="C13" s="432">
+        <f>'Data Summaries'!F124</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D13" s="434">
+        <f>'Data Summaries'!I124</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E13" s="432">
+        <f>'Data Summaries'!L124</f>
+        <v>0.09</v>
+      </c>
+      <c r="F13" s="434">
+        <f>'Data Summaries'!O124</f>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G13" s="432">
+        <f>'Data Summaries'!R124</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="432">
+        <f>'Data Summaries'!AA124</f>
+        <v>0.53</v>
+      </c>
+      <c r="I13" s="439">
+        <f>'Data Summaries'!S50</f>
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="302" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>617</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>631</v>
+      </c>
+      <c r="B18" s="432">
+        <f>'Data Summaries'!AH64</f>
+        <v>3.7176808603425524</v>
+      </c>
+      <c r="C18" s="432">
+        <f>'Data Summaries'!AH65</f>
+        <v>4.2874609699645481</v>
+      </c>
+      <c r="D18" s="432">
+        <f>'Data Summaries'!AH66</f>
+        <v>2.7353973412185391</v>
+      </c>
+      <c r="E18" s="432">
+        <f>'Data Summaries'!AH67</f>
+        <v>1.2432254956452389</v>
+      </c>
+      <c r="F18" s="432">
+        <f>'Data Summaries'!AH68</f>
+        <v>0.40987377896792981</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>632</v>
+      </c>
+      <c r="B19" s="432">
+        <f>'Data Summaries'!AD64</f>
+        <v>6.7128897072221099</v>
+      </c>
+      <c r="C19" s="432">
+        <f>'Data Summaries'!AD65</f>
+        <v>7.8751824899390703</v>
+      </c>
+      <c r="D19" s="432">
+        <f>'Data Summaries'!AD66</f>
+        <v>5.0912943385710738</v>
+      </c>
+      <c r="E19" s="432">
+        <f>'Data Summaries'!AD67</f>
+        <v>2.3430468084648366</v>
+      </c>
+      <c r="F19" s="432">
+        <f>'Data Summaries'!AD68</f>
+        <v>0.84259923379982948</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>633</v>
+      </c>
+      <c r="B20" s="432">
+        <f>'Data Summaries'!AF64</f>
+        <v>0.65853873538669128</v>
+      </c>
+      <c r="C20" s="432">
+        <f>'Data Summaries'!AF65</f>
+        <v>0.72850016807037643</v>
+      </c>
+      <c r="D20" s="432">
+        <f>'Data Summaries'!AF66</f>
+        <v>0.44433647990292957</v>
+      </c>
+      <c r="E20" s="432">
+        <f>'Data Summaries'!AF67</f>
+        <v>0.18011984146852941</v>
+      </c>
+      <c r="F20" s="432">
+        <f>'Data Summaries'!AF68</f>
+        <v>2.1724961981316532E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>634</v>
+      </c>
+      <c r="B21" s="214">
+        <f>'Data Summaries'!N64</f>
+        <v>2.5029102745667955</v>
+      </c>
+      <c r="C21" s="214">
+        <f>'Data Summaries'!N65</f>
+        <v>3.1833932632033419</v>
+      </c>
+      <c r="D21" s="214">
+        <f>'Data Summaries'!N66</f>
+        <v>2.1526494734645469</v>
+      </c>
+      <c r="E21" s="214">
+        <f>'Data Summaries'!N67</f>
+        <v>1.0545130486689225</v>
+      </c>
+      <c r="F21" s="214">
+        <f>'Data Summaries'!N68</f>
+        <v>0.38957824344718012</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>635</v>
+      </c>
+      <c r="B22" s="214">
+        <f>'Data Summaries'!Y64</f>
+        <v>33.680822268554081</v>
+      </c>
+      <c r="C22" s="214">
+        <f>'Data Summaries'!Y65</f>
+        <v>43.106197512490702</v>
+      </c>
+      <c r="D22" s="214">
+        <f>'Data Summaries'!Y66</f>
+        <v>23.519934647938459</v>
+      </c>
+      <c r="E22" s="214">
+        <f>'Data Summaries'!Y67</f>
+        <v>9.5004143482893344</v>
+      </c>
+      <c r="F22" s="214">
+        <f>'Data Summaries'!Y68</f>
+        <v>2.1794599192005104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>636</v>
+      </c>
+      <c r="B23" s="432">
+        <f>'Data Summaries'!J64</f>
+        <v>4.54394625023125</v>
+      </c>
+      <c r="C23" s="432">
+        <f>'Data Summaries'!J65</f>
+        <v>5.9002582614844421</v>
+      </c>
+      <c r="D23" s="432">
+        <f>'Data Summaries'!J66</f>
+        <v>4.0258609185925156</v>
+      </c>
+      <c r="E23" s="432">
+        <f>'Data Summaries'!J67</f>
+        <v>1.9835990393467668</v>
+      </c>
+      <c r="F23" s="432">
+        <f>'Data Summaries'!J68</f>
+        <v>0.80044202617097404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>637</v>
+      </c>
+      <c r="B24" s="432">
+        <f>'Data Summaries'!L64</f>
+        <v>0.42061870494975945</v>
+      </c>
+      <c r="C24" s="432">
+        <f>'Data Summaries'!L65</f>
+        <v>0.48676986027054281</v>
+      </c>
+      <c r="D24" s="432">
+        <f>'Data Summaries'!L66</f>
+        <v>0.32781799444467818</v>
+      </c>
+      <c r="E24" s="432">
+        <f>'Data Summaries'!L67</f>
+        <v>0.1550864357276549</v>
+      </c>
+      <c r="F24" s="432">
+        <f>'Data Summaries'!L68</f>
+        <v>2.0823355475501321E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>638</v>
+      </c>
+      <c r="B25" s="432">
+        <f>'Data Summaries'!U64</f>
+        <v>59.468030398262954</v>
+      </c>
+      <c r="C25" s="432">
+        <f>'Data Summaries'!U65</f>
+        <v>78.039418639755027</v>
+      </c>
+      <c r="D25" s="432">
+        <f>'Data Summaries'!U66</f>
+        <v>44.360491363128752</v>
+      </c>
+      <c r="E25" s="432">
+        <f>'Data Summaries'!U67</f>
+        <v>18.629863858687187</v>
+      </c>
+      <c r="F25" s="432">
+        <f>'Data Summaries'!U68</f>
+        <v>4.621072088724584</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>639</v>
+      </c>
+      <c r="B26" s="432">
+        <f>'Data Summaries'!W64</f>
+        <v>6.6125864059618236</v>
+      </c>
+      <c r="C26" s="432">
+        <f>'Data Summaries'!W65</f>
+        <v>9.1412277759141229</v>
+      </c>
+      <c r="D26" s="432">
+        <f>'Data Summaries'!W66</f>
+        <v>4.4733013398188959</v>
+      </c>
+      <c r="E26" s="432">
+        <f>'Data Summaries'!W67</f>
+        <v>1.240240155593765</v>
+      </c>
+      <c r="F26" s="432">
+        <f>'Data Summaries'!W68</f>
+        <v>9.8463962189838522E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>618</v>
+      </c>
+      <c r="B28" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>640</v>
+      </c>
+      <c r="B29" s="26">
+        <f>'Data Summaries'!M63</f>
+        <v>376</v>
+      </c>
+      <c r="C29" s="26">
+        <f>'Data Summaries'!M64</f>
+        <v>8439</v>
+      </c>
+      <c r="D29" s="26">
+        <f>'Data Summaries'!M65</f>
+        <v>10529</v>
+      </c>
+      <c r="E29" s="26">
+        <f>'Data Summaries'!M66</f>
+        <v>6767</v>
+      </c>
+      <c r="F29" s="26">
+        <f>'Data Summaries'!M67</f>
+        <v>3118</v>
+      </c>
+      <c r="G29" s="26">
+        <f>'Data Summaries'!M68</f>
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>641</v>
+      </c>
+      <c r="B30" s="26">
+        <f>'Data Summaries'!X63</f>
+        <v>378</v>
+      </c>
+      <c r="C30" s="26">
+        <f>'Data Summaries'!X64</f>
+        <v>4604</v>
+      </c>
+      <c r="D30" s="26">
+        <f>'Data Summaries'!X65</f>
+        <v>4055</v>
+      </c>
+      <c r="E30" s="26">
+        <f>'Data Summaries'!X66</f>
+        <v>2073</v>
+      </c>
+      <c r="F30" s="26">
+        <f>'Data Summaries'!X67</f>
+        <v>642</v>
+      </c>
+      <c r="G30" s="26">
+        <f>'Data Summaries'!X68</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>642</v>
+      </c>
+      <c r="B31" s="26">
+        <f>'Data Summaries'!I63</f>
+        <v>353</v>
+      </c>
+      <c r="C31" s="26">
+        <f>'Data Summaries'!I64</f>
+        <v>7737</v>
+      </c>
+      <c r="D31" s="26">
+        <f>'Data Summaries'!I65</f>
+        <v>9721</v>
+      </c>
+      <c r="E31" s="26">
+        <f>'Data Summaries'!I66</f>
+        <v>6245</v>
+      </c>
+      <c r="F31" s="26">
+        <f>'Data Summaries'!I67</f>
+        <v>2885</v>
+      </c>
+      <c r="G31" s="26">
+        <f>'Data Summaries'!I68</f>
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>643</v>
+      </c>
+      <c r="B32" s="26">
+        <f>'Data Summaries'!K63</f>
+        <v>23</v>
+      </c>
+      <c r="C32" s="26">
+        <f>'Data Summaries'!K64</f>
+        <v>702</v>
+      </c>
+      <c r="D32" s="26">
+        <f>'Data Summaries'!K65</f>
+        <v>808</v>
+      </c>
+      <c r="E32" s="26">
+        <f>'Data Summaries'!K66</f>
+        <v>522</v>
+      </c>
+      <c r="F32" s="26">
+        <f>'Data Summaries'!K67</f>
+        <v>233</v>
+      </c>
+      <c r="G32" s="26">
+        <f>'Data Summaries'!K68</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>644</v>
+      </c>
+      <c r="B33" s="26">
+        <f>'Data Summaries'!T63</f>
+        <v>348</v>
+      </c>
+      <c r="C33" s="26">
+        <f>'Data Summaries'!T64</f>
+        <v>4163</v>
+      </c>
+      <c r="D33" s="26">
+        <f>'Data Summaries'!T65</f>
+        <v>3619</v>
+      </c>
+      <c r="E33" s="26">
+        <f>'Data Summaries'!T66</f>
+        <v>1867</v>
+      </c>
+      <c r="F33" s="26">
+        <f>'Data Summaries'!T67</f>
+        <v>598</v>
+      </c>
+      <c r="G33" s="26">
+        <f>'Data Summaries'!T68</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>645</v>
+      </c>
+      <c r="B34" s="26">
+        <f>'Data Summaries'!V63</f>
+        <v>30</v>
+      </c>
+      <c r="C34" s="26">
+        <f>'Data Summaries'!V64</f>
+        <v>441</v>
+      </c>
+      <c r="D34" s="26">
+        <f>'Data Summaries'!V65</f>
+        <v>436</v>
+      </c>
+      <c r="E34" s="26">
+        <f>'Data Summaries'!V66</f>
+        <v>206</v>
+      </c>
+      <c r="F34" s="26">
+        <f>'Data Summaries'!V67</f>
+        <v>44</v>
+      </c>
+      <c r="G34" s="26">
+        <f>'Data Summaries'!V68</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>646</v>
+      </c>
+      <c r="B35" s="26">
+        <f>'Data Summaries'!AG63</f>
+        <v>754</v>
+      </c>
+      <c r="C35" s="26">
+        <f>'Data Summaries'!AG64</f>
+        <v>13043</v>
+      </c>
+      <c r="D35" s="26">
+        <f>'Data Summaries'!AG65</f>
+        <v>14584</v>
+      </c>
+      <c r="E35" s="26">
+        <f>'Data Summaries'!AG66</f>
+        <v>8840</v>
+      </c>
+      <c r="F35" s="26">
+        <f>'Data Summaries'!AG67</f>
+        <v>3760</v>
+      </c>
+      <c r="G35" s="26">
+        <f>'Data Summaries'!AG68</f>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="301" customFormat="1">
+      <c r="A36" s="301" t="s">
+        <v>655</v>
+      </c>
+      <c r="B36" s="26">
+        <f>'Data Summaries'!AC63</f>
+        <v>701</v>
+      </c>
+      <c r="C36" s="26">
+        <f>'Data Summaries'!AC64</f>
+        <v>11900</v>
+      </c>
+      <c r="D36" s="26">
+        <f>'Data Summaries'!AC65</f>
+        <v>13340</v>
+      </c>
+      <c r="E36" s="26">
+        <f>'Data Summaries'!AC66</f>
+        <v>8112</v>
+      </c>
+      <c r="F36" s="26">
+        <f>'Data Summaries'!AC67</f>
+        <v>3483</v>
+      </c>
+      <c r="G36" s="26">
+        <f>'Data Summaries'!AC68</f>
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="301" customFormat="1">
+      <c r="A37" s="301" t="s">
+        <v>656</v>
+      </c>
+      <c r="B37" s="26">
+        <f>'Data Summaries'!AE63</f>
+        <v>53</v>
+      </c>
+      <c r="C37" s="26">
+        <f>'Data Summaries'!AE64</f>
+        <v>1143</v>
+      </c>
+      <c r="D37" s="26">
+        <f>'Data Summaries'!AE65</f>
+        <v>1244</v>
+      </c>
+      <c r="E37" s="26">
+        <f>'Data Summaries'!AE66</f>
+        <v>728</v>
+      </c>
+      <c r="F37" s="26">
+        <f>'Data Summaries'!AE67</f>
+        <v>277</v>
+      </c>
+      <c r="G37" s="26">
+        <f>'Data Summaries'!AE68</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>630</v>
+      </c>
+      <c r="B39" t="s">
+        <v>619</v>
+      </c>
+      <c r="C39" s="435" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>647</v>
+      </c>
+      <c r="B40" s="433">
+        <f>'Data Summaries'!E61</f>
+        <v>0.13063764398783725</v>
+      </c>
+      <c r="C40" s="433">
+        <f>'Data Summaries'!E62</f>
+        <v>0.12109420846479671</v>
+      </c>
+      <c r="D40" s="433">
+        <f>'Data Summaries'!E64</f>
+        <v>0.14672640031656342</v>
+      </c>
+      <c r="E40" s="433">
+        <f>'Data Summaries'!E65</f>
+        <v>0.14197398520210819</v>
+      </c>
+      <c r="F40" s="433">
+        <f>'Data Summaries'!E66</f>
+        <v>0.13367264054869152</v>
+      </c>
+      <c r="G40" s="433">
+        <f>'Data Summaries'!E67</f>
+        <v>0.12533165653076628</v>
+      </c>
+      <c r="H40" s="433">
+        <f>'Data Summaries'!E69</f>
+        <v>0.10415777294330726</v>
+      </c>
+      <c r="I40" s="433">
+        <f>'Data Summaries'!E70</f>
+        <v>9.6405692005929355E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>648</v>
+      </c>
+      <c r="B41" s="433">
+        <f>'Data Summaries'!G61</f>
+        <v>0.12192299300402208</v>
+      </c>
+      <c r="C41" s="433">
+        <f>'Data Summaries'!G62</f>
+        <v>0.11315223148858543</v>
+      </c>
+      <c r="D41" s="433">
+        <f>'Data Summaries'!G64</f>
+        <v>0.14158312631342129</v>
+      </c>
+      <c r="E41" s="433">
+        <f>'Data Summaries'!G65</f>
+        <v>0.14081556061308886</v>
+      </c>
+      <c r="F41" s="433">
+        <f>'Data Summaries'!G66</f>
+        <v>0.13508299516216438</v>
+      </c>
+      <c r="G41" s="433">
+        <f>'Data Summaries'!G67</f>
+        <v>0.12745153596276051</v>
+      </c>
+      <c r="H41" s="433">
+        <f>'Data Summaries'!G69</f>
+        <v>0.1061605800380661</v>
+      </c>
+      <c r="I41" s="433">
+        <f>'Data Summaries'!G70</f>
+        <v>0.11383097741789133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>649</v>
+      </c>
+      <c r="B42" s="433">
+        <f>'Data Summaries'!P61</f>
+        <v>0.24123459826863078</v>
+      </c>
+      <c r="C42" s="433">
+        <f>'Data Summaries'!P62</f>
+        <v>0.21527911990823592</v>
+      </c>
+      <c r="D42" s="433">
+        <f>'Data Summaries'!P64</f>
+        <v>0.17570711799062783</v>
+      </c>
+      <c r="E42" s="433">
+        <f>'Data Summaries'!P65</f>
+        <v>0.11639680432114415</v>
+      </c>
+      <c r="F42" s="433">
+        <f>'Data Summaries'!P66</f>
+        <v>0.10563661326312143</v>
+      </c>
+      <c r="G42" s="433">
+        <f>'Data Summaries'!P67</f>
+        <v>8.0567150168292703E-2</v>
+      </c>
+      <c r="H42" s="433">
+        <f>'Data Summaries'!P69</f>
+        <v>4.5139089336944327E-2</v>
+      </c>
+      <c r="I42" s="433">
+        <f>'Data Summaries'!P70</f>
+        <v>2.0039506743002863E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>650</v>
+      </c>
+      <c r="B43" s="433">
+        <f>'Data Summaries'!R61</f>
+        <v>0.22896997639716765</v>
+      </c>
+      <c r="C43" s="433">
+        <f>'Data Summaries'!R62</f>
+        <v>0.20500460055206624</v>
+      </c>
+      <c r="D43" s="433">
+        <f>'Data Summaries'!R64</f>
+        <v>0.16674750970116414</v>
+      </c>
+      <c r="E43" s="433">
+        <f>'Data Summaries'!R65</f>
+        <v>0.11925431051726207</v>
+      </c>
+      <c r="F43" s="433">
+        <f>'Data Summaries'!R66</f>
+        <v>0.11514131695803496</v>
+      </c>
+      <c r="G43" s="433">
+        <f>'Data Summaries'!R67</f>
+        <v>8.870314437732528E-2</v>
+      </c>
+      <c r="H43" s="433">
+        <f>'Data Summaries'!R69</f>
+        <v>4.9645957514901785E-2</v>
+      </c>
+      <c r="I43" s="433">
+        <f>'Data Summaries'!R70</f>
+        <v>2.6533183982077848E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>651</v>
+      </c>
+      <c r="B44" s="26">
+        <f>'Data Summaries'!D61</f>
+        <v>1516001</v>
+      </c>
+      <c r="C44" s="26">
+        <f>'Data Summaries'!D62</f>
+        <v>1405253</v>
+      </c>
+      <c r="D44" s="26">
+        <f>'Data Summaries'!D64</f>
+        <v>1702705</v>
+      </c>
+      <c r="E44" s="26">
+        <f>'Data Summaries'!D65</f>
+        <v>1647555</v>
+      </c>
+      <c r="F44" s="26">
+        <f>'Data Summaries'!D66</f>
+        <v>1551221</v>
+      </c>
+      <c r="G44" s="26">
+        <f>'Data Summaries'!D67</f>
+        <v>1454427</v>
+      </c>
+      <c r="H44" s="26">
+        <f>'Data Summaries'!D69</f>
+        <v>1208712</v>
+      </c>
+      <c r="I44" s="26">
+        <f>'Data Summaries'!D70</f>
+        <v>1118752</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>652</v>
+      </c>
+      <c r="B45" s="26">
+        <f>'Data Summaries'!F61</f>
+        <v>1437218</v>
+      </c>
+      <c r="C45" s="26">
+        <f>'Data Summaries'!F62</f>
+        <v>1333829</v>
+      </c>
+      <c r="D45" s="26">
+        <f>'Data Summaries'!F64</f>
+        <v>1668970</v>
+      </c>
+      <c r="E45" s="26">
+        <f>'Data Summaries'!F65</f>
+        <v>1659922</v>
+      </c>
+      <c r="F45" s="26">
+        <f>'Data Summaries'!F66</f>
+        <v>1592347</v>
+      </c>
+      <c r="G45" s="26">
+        <f>'Data Summaries'!F67</f>
+        <v>1502388</v>
+      </c>
+      <c r="H45" s="26">
+        <f>'Data Summaries'!F69</f>
+        <v>1251412</v>
+      </c>
+      <c r="I45" s="26">
+        <f>'Data Summaries'!F70</f>
+        <v>1341830</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>653</v>
+      </c>
+      <c r="B46" s="26">
+        <f>'Data Summaries'!O61</f>
+        <v>96111</v>
+      </c>
+      <c r="C46" s="26">
+        <f>'Data Summaries'!O62</f>
+        <v>85770</v>
+      </c>
+      <c r="D46" s="26">
+        <f>'Data Summaries'!O64</f>
+        <v>70004</v>
+      </c>
+      <c r="E46" s="26">
+        <f>'Data Summaries'!O65</f>
+        <v>46374</v>
+      </c>
+      <c r="F46" s="26">
+        <f>'Data Summaries'!O66</f>
+        <v>42087</v>
+      </c>
+      <c r="G46" s="26">
+        <f>'Data Summaries'!O67</f>
+        <v>32099</v>
+      </c>
+      <c r="H46" s="26">
+        <f>'Data Summaries'!O69</f>
+        <v>17984</v>
+      </c>
+      <c r="I46" s="26">
+        <f>'Data Summaries'!O70</f>
+        <v>7984</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>654</v>
+      </c>
+      <c r="B47" s="26">
+        <f>'Data Summaries'!Q61</f>
+        <v>91577</v>
+      </c>
+      <c r="C47" s="26">
+        <f>'Data Summaries'!Q62</f>
+        <v>81992</v>
+      </c>
+      <c r="D47" s="26">
+        <f>'Data Summaries'!Q64</f>
+        <v>66691</v>
+      </c>
+      <c r="E47" s="26">
+        <f>'Data Summaries'!Q65</f>
+        <v>47696</v>
+      </c>
+      <c r="F47" s="26">
+        <f>'Data Summaries'!Q66</f>
+        <v>46051</v>
+      </c>
+      <c r="G47" s="26">
+        <f>'Data Summaries'!Q67</f>
+        <v>35477</v>
+      </c>
+      <c r="H47" s="26">
+        <f>'Data Summaries'!Q69</f>
+        <v>19856</v>
+      </c>
+      <c r="I47" s="26">
+        <f>'Data Summaries'!Q70</f>
+        <v>10612</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="301" customFormat="1"/>
+    <row r="49" spans="1:9" s="301" customFormat="1">
+      <c r="A49" s="301" t="s">
+        <v>657</v>
+      </c>
+      <c r="B49" s="214">
+        <f>'Data Summaries'!AI63</f>
+        <v>1.7383944094320523</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="301" customFormat="1">
+      <c r="A50" s="301" t="s">
+        <v>658</v>
+      </c>
+      <c r="B50" s="214">
+        <f>'Data Summaries'!AI70</f>
+        <v>25.957576510165605</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="302" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="301" t="s">
+        <v>621</v>
+      </c>
+      <c r="B53" s="301" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="301" t="s">
+        <v>525</v>
+      </c>
+      <c r="E53" s="301" t="s">
+        <v>173</v>
+      </c>
+      <c r="F53" s="301" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="301" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="301" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="301" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="301" t="s">
+        <v>623</v>
+      </c>
+      <c r="B54" s="432">
+        <f>'Data Summaries'!C116</f>
+        <v>0.04</v>
+      </c>
+      <c r="C54" s="432">
+        <f>'Data Summaries'!F116</f>
+        <v>0.06</v>
+      </c>
+      <c r="D54" s="433">
+        <f>'Data Summaries'!I116</f>
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E54" s="432">
+        <f>'Data Summaries'!L116</f>
+        <v>0.13</v>
+      </c>
+      <c r="F54" s="432">
+        <f>'Data Summaries'!O116</f>
+        <v>0.36</v>
+      </c>
+      <c r="G54" s="432">
+        <f>'Data Summaries'!R116</f>
+        <v>0.01</v>
+      </c>
+      <c r="H54" s="432">
+        <f>'Data Summaries'!AA116</f>
+        <v>0.74</v>
+      </c>
+      <c r="I54" s="439">
+        <f>'Data Summaries'!V55</f>
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="301" t="s">
+        <v>624</v>
+      </c>
+      <c r="B55" s="432">
+        <f>'Data Summaries'!C117</f>
+        <v>0.03</v>
+      </c>
+      <c r="C55" s="432">
+        <f>'Data Summaries'!F117</f>
+        <v>0.03</v>
+      </c>
+      <c r="D55" s="433">
+        <f>'Data Summaries'!I117</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E55" s="432">
+        <f>'Data Summaries'!L117</f>
+        <v>0.27</v>
+      </c>
+      <c r="F55" s="433">
+        <f>'Data Summaries'!O117</f>
+        <v>0.314</v>
+      </c>
+      <c r="G55" s="432">
+        <f>'Data Summaries'!R117</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="432">
+        <f>'Data Summaries'!AA117</f>
+        <v>0.86</v>
+      </c>
+      <c r="I55" s="439">
+        <f>'Data Summaries'!Y55</f>
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="301" t="s">
+        <v>659</v>
+      </c>
+      <c r="B56" s="432">
+        <f>'Data Summaries'!C118</f>
+        <v>0.05</v>
+      </c>
+      <c r="C56" s="432">
+        <f>'Data Summaries'!F118</f>
+        <v>0.09</v>
+      </c>
+      <c r="D56" s="433">
+        <f>'Data Summaries'!I118</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E56" s="432">
+        <f>'Data Summaries'!L118</f>
+        <v>0.11</v>
+      </c>
+      <c r="F56" s="433">
+        <f>'Data Summaries'!O118</f>
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G56" s="432">
+        <f>'Data Summaries'!R118</f>
+        <v>0.01</v>
+      </c>
+      <c r="H56" s="432">
+        <f>'Data Summaries'!AA118</f>
+        <v>0.8</v>
+      </c>
+      <c r="I56" s="439">
+        <f>'Data Summaries'!J55</f>
+        <v>0.72400000000000009</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="301" t="s">
+        <v>660</v>
+      </c>
+      <c r="B57" s="432">
+        <f>'Data Summaries'!C119</f>
+        <v>0.03</v>
+      </c>
+      <c r="C57" s="432">
+        <f>'Data Summaries'!F119</f>
+        <v>0.04</v>
+      </c>
+      <c r="D57" s="433">
+        <f>'Data Summaries'!I119</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E57" s="432">
+        <f>'Data Summaries'!L119</f>
+        <v>0.19</v>
+      </c>
+      <c r="F57" s="433">
+        <f>'Data Summaries'!O119</f>
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G57" s="432">
+        <f>'Data Summaries'!R119</f>
+        <v>0.01</v>
+      </c>
+      <c r="H57" s="432">
+        <f>'Data Summaries'!AA119</f>
+        <v>0.73</v>
+      </c>
+      <c r="I57" s="439">
+        <f>'Data Summaries'!S55</f>
+        <v>0.626</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="301" t="s">
+        <v>617</v>
+      </c>
+      <c r="B59" s="301" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="301" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" s="301" t="s">
+        <v>205</v>
+      </c>
+      <c r="E59" s="301" t="s">
+        <v>206</v>
+      </c>
+      <c r="F59" s="301" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>661</v>
+      </c>
+      <c r="B60" s="26">
+        <f>'Data Summaries'!AG76</f>
+        <v>6048.3481676905894</v>
+      </c>
+      <c r="C60" s="26">
+        <f>'Data Summaries'!AG77</f>
+        <v>15521.901451053342</v>
+      </c>
+      <c r="D60" s="26">
+        <f>'Data Summaries'!AG78</f>
+        <v>11885.752374017402</v>
+      </c>
+      <c r="E60" s="26">
+        <f>'Data Summaries'!AG79</f>
+        <v>6122.6429837205578</v>
+      </c>
+      <c r="F60" s="26">
+        <f>'Data Summaries'!AG80</f>
+        <v>3468.0717639909399</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>662</v>
+      </c>
+      <c r="B61" s="433">
+        <f>'Data Summaries'!J20</f>
+        <v>0</v>
+      </c>
+      <c r="C61" s="433">
+        <f>'Data Summaries'!J21</f>
+        <v>8.8652482269503544E-4</v>
+      </c>
+      <c r="D61" s="433">
+        <f>'Data Summaries'!J22</f>
+        <v>1.1061946902654867E-3</v>
+      </c>
+      <c r="E61" s="433">
+        <f>'Data Summaries'!J23</f>
+        <v>1.7730496453900709E-3</v>
+      </c>
+      <c r="F61" s="433">
+        <f>'Data Summaries'!J24</f>
+        <v>8.6132644272179162E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>663</v>
+      </c>
+      <c r="B62" s="433">
+        <f>'Data Summaries'!K20</f>
+        <v>2E-3</v>
+      </c>
+      <c r="C62" s="433">
+        <f>'Data Summaries'!K21</f>
+        <v>2E-3</v>
+      </c>
+      <c r="D62" s="433">
+        <f>'Data Summaries'!K22</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E62" s="433">
+        <f>'Data Summaries'!K23</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F62" s="433">
+        <f>'Data Summaries'!K24</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>664</v>
+      </c>
+      <c r="B63" s="433">
+        <f>'Data Summaries'!L20</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="433">
+        <f>'Data Summaries'!L21</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D63" s="433">
+        <f>'Data Summaries'!L22</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E63" s="433">
+        <f>'Data Summaries'!L23</f>
+        <v>0.01</v>
+      </c>
+      <c r="F63" s="433">
+        <f>'Data Summaries'!L24</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>665</v>
+      </c>
+      <c r="B64" s="433">
+        <f>'Data Summaries'!N20</f>
+        <v>0</v>
+      </c>
+      <c r="C64" s="433">
+        <f>'Data Summaries'!N21</f>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D64" s="433">
+        <f>'Data Summaries'!N22</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E64" s="433">
+        <f>'Data Summaries'!N23</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F64" s="433">
+        <f>'Data Summaries'!N24</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>666</v>
+      </c>
+      <c r="B65" s="433">
+        <f>'Data Summaries'!M20</f>
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="C65" s="433">
+        <f>'Data Summaries'!M21</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="D65" s="433">
+        <f>'Data Summaries'!M22</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E65" s="433">
+        <f>'Data Summaries'!M23</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F65" s="433">
+        <f>'Data Summaries'!M24</f>
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>625</v>
+      </c>
+      <c r="B67" s="432">
+        <f>'Data Summaries'!C120</f>
+        <v>0.01</v>
+      </c>
+      <c r="C67" s="432">
+        <f>'Data Summaries'!F120</f>
+        <v>0.01</v>
+      </c>
+      <c r="D67">
+        <f>'Data Summaries'!I120</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="432">
+        <f>'Data Summaries'!L120</f>
+        <v>0.18</v>
+      </c>
+      <c r="F67">
+        <f>'Data Summaries'!O120</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G67" s="432">
+        <f>'Data Summaries'!G90</f>
+        <v>0.01</v>
+      </c>
+      <c r="H67" s="432">
+        <f>'Data Summaries'!I90</f>
+        <v>0.8</v>
+      </c>
+      <c r="I67">
+        <f>'Data Summaries'!AB46</f>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>626</v>
+      </c>
+      <c r="B68" s="432">
+        <f>'Data Summaries'!C121</f>
+        <v>0.02</v>
+      </c>
+      <c r="C68" s="432">
+        <f>'Data Summaries'!F121</f>
+        <v>0.03</v>
+      </c>
+      <c r="D68" s="301">
+        <f>'Data Summaries'!I121</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="432">
+        <f>'Data Summaries'!L121</f>
+        <v>0.15</v>
+      </c>
+      <c r="F68" s="301">
+        <f>'Data Summaries'!O121</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G68" s="432">
+        <f>'Data Summaries'!G91</f>
+        <v>0.01</v>
+      </c>
+      <c r="H68" s="432">
+        <f>'Data Summaries'!I91</f>
+        <v>0.76</v>
+      </c>
+      <c r="I68" s="301">
+        <f>'Data Summaries'!AB47</f>
+        <v>0.57700000000000007</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>627</v>
+      </c>
+      <c r="B69" s="432">
+        <f>'Data Summaries'!C122</f>
+        <v>0.04</v>
+      </c>
+      <c r="C69" s="432">
+        <f>'Data Summaries'!F122</f>
+        <v>0.08</v>
+      </c>
+      <c r="D69" s="301">
+        <f>'Data Summaries'!I122</f>
+        <v>0</v>
+      </c>
+      <c r="E69" s="432">
+        <f>'Data Summaries'!L122</f>
+        <v>0.15</v>
+      </c>
+      <c r="F69" s="301">
+        <f>'Data Summaries'!O122</f>
+        <v>0.159</v>
+      </c>
+      <c r="G69" s="432">
+        <f>'Data Summaries'!G92</f>
+        <v>0</v>
+      </c>
+      <c r="H69" s="432">
+        <f>'Data Summaries'!I92</f>
+        <v>0.79</v>
+      </c>
+      <c r="I69" s="301">
+        <f>'Data Summaries'!AB48</f>
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>628</v>
+      </c>
+      <c r="B70" s="432">
+        <f>'Data Summaries'!C123</f>
+        <v>0.04</v>
+      </c>
+      <c r="C70" s="432">
+        <f>'Data Summaries'!F123</f>
+        <v>0.08</v>
+      </c>
+      <c r="D70" s="301">
+        <f>'Data Summaries'!I123</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E70" s="432">
+        <f>'Data Summaries'!L123</f>
+        <v>0.18</v>
+      </c>
+      <c r="F70" s="301">
+        <f>'Data Summaries'!O123</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="G70" s="432">
+        <f>'Data Summaries'!G93</f>
+        <v>0.03</v>
+      </c>
+      <c r="H70" s="432">
+        <f>'Data Summaries'!I93</f>
+        <v>0.66</v>
+      </c>
+      <c r="I70" s="301">
+        <f>'Data Summaries'!AB49</f>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>629</v>
+      </c>
+      <c r="B71" s="432">
+        <f>'Data Summaries'!C124</f>
+        <v>0.38</v>
+      </c>
+      <c r="C71" s="432">
+        <f>'Data Summaries'!F124</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D71" s="301">
+        <f>'Data Summaries'!I124</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E71" s="432">
+        <f>'Data Summaries'!L124</f>
+        <v>0.09</v>
+      </c>
+      <c r="F71" s="301">
+        <f>'Data Summaries'!O124</f>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G71" s="432">
+        <f>'Data Summaries'!G94</f>
+        <v>0</v>
+      </c>
+      <c r="H71" s="432">
+        <f>'Data Summaries'!I94</f>
+        <v>0.53</v>
+      </c>
+      <c r="I71" s="437">
+        <f>'Data Summaries'!S50</f>
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>667</v>
+      </c>
+      <c r="B72" s="433">
+        <f>'Data Summaries'!C32</f>
+        <v>0.105</v>
+      </c>
+      <c r="C72" s="433">
+        <f>'Data Summaries'!C33</f>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="D72" s="433">
+        <f>'Data Summaries'!C34</f>
+        <v>6.3E-2</v>
+      </c>
+      <c r="E72" s="433">
+        <f>'Data Summaries'!C35</f>
+        <v>0</v>
+      </c>
+      <c r="F72" s="433">
+        <f>'Data Summaries'!C36</f>
+        <v>0.06</v>
+      </c>
+      <c r="G72" s="433">
+        <f>'Data Summaries'!C37</f>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H72" s="437">
+        <v>0</v>
+      </c>
+      <c r="I72" s="437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>655</v>
+      </c>
+      <c r="B74" s="26">
+        <f>SUM('Data Summaries'!AC63:AC68)</f>
+        <v>39519</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>656</v>
+      </c>
+      <c r="B75" s="26">
+        <f>SUM('Data Summaries'!AE63:AE68)</f>
+        <v>3502</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>668</v>
+      </c>
+      <c r="B76">
+        <f>'Data Summaries'!B137*(1-'Data Summaries'!B139)</f>
+        <v>18290.000000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>669</v>
+      </c>
+      <c r="B77">
+        <f>'Data Summaries'!B137*'Data Summaries'!B139</f>
+        <v>12710</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>670</v>
+      </c>
+      <c r="B78" s="440">
+        <f>SUM('Data Summaries'!X76:X80)</f>
+        <v>12110.520078583319</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>671</v>
+      </c>
+      <c r="B79" s="438">
+        <f>SUM('Data Summaries'!S75:S80)</f>
+        <v>798365</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>672</v>
+      </c>
+      <c r="B80" s="440">
+        <f>SUM('Data Summaries'!M76:M80)</f>
+        <v>31164.774226242287</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>673</v>
+      </c>
+      <c r="B81" s="440">
+        <f>SUM('Data Summaries'!H75:H80)</f>
+        <v>23392542</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="301" customFormat="1">
+      <c r="B82" s="438"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>674</v>
+      </c>
+      <c r="B84" s="433">
+        <f>'Data Summaries'!C98</f>
+        <v>1.6057585825027684E-2</v>
+      </c>
+      <c r="C84" s="433">
+        <f>'Data Summaries'!C99</f>
+        <v>1.2842465753424657E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>675</v>
+      </c>
+      <c r="B85" s="433">
+        <f>'Data Summaries'!F98</f>
+        <v>3.5327999999999998E-2</v>
+      </c>
+      <c r="C85" s="433">
+        <f>'Data Summaries'!F99</f>
+        <v>1.9871999999999997E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>676</v>
+      </c>
+      <c r="B86" s="433">
+        <f>'Data Summaries'!H98</f>
+        <v>8.6241999999999999E-2</v>
+      </c>
+      <c r="C86" s="433">
+        <f>'Data Summaries'!H99</f>
+        <v>5.2858000000000002E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>677</v>
+      </c>
+      <c r="B87" s="433">
+        <f>'Data Summaries'!L98</f>
+        <v>1.2272E-2</v>
+      </c>
+      <c r="C87" s="433">
+        <f>'Data Summaries'!L99</f>
+        <v>1.1328E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>678</v>
+      </c>
+      <c r="B88" s="433">
+        <f>'Data Summaries'!J98</f>
+        <v>6.8323999999999996E-2</v>
+      </c>
+      <c r="C88" s="433">
+        <f>'Data Summaries'!J99</f>
+        <v>4.9475999999999999E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>618</v>
+      </c>
+      <c r="B90" s="301" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="301" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" s="301" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="301" t="s">
+        <v>5</v>
+      </c>
+      <c r="F90" s="301" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>684</v>
+      </c>
+      <c r="B91" s="26">
+        <f>'Data Summaries'!AG64</f>
+        <v>13043</v>
+      </c>
+      <c r="C91" s="26">
+        <f>'Data Summaries'!AG65</f>
+        <v>14584</v>
+      </c>
+      <c r="D91" s="26">
+        <f>'Data Summaries'!AG66</f>
+        <v>8840</v>
+      </c>
+      <c r="E91" s="26">
+        <f>'Data Summaries'!AG67</f>
+        <v>3760</v>
+      </c>
+      <c r="F91" s="26">
+        <f>'Data Summaries'!AG68</f>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>679</v>
+      </c>
+      <c r="B92" s="433">
+        <f>'Data Summaries'!J20</f>
+        <v>0</v>
+      </c>
+      <c r="C92" s="433">
+        <f>'Data Summaries'!J21</f>
+        <v>8.8652482269503544E-4</v>
+      </c>
+      <c r="D92" s="433">
+        <f>'Data Summaries'!J22</f>
+        <v>1.1061946902654867E-3</v>
+      </c>
+      <c r="E92" s="433">
+        <f>'Data Summaries'!J23</f>
+        <v>1.7730496453900709E-3</v>
+      </c>
+      <c r="F92" s="433">
+        <f>'Data Summaries'!J24</f>
+        <v>8.6132644272179162E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>680</v>
+      </c>
+      <c r="B93" s="433">
+        <f>'Data Summaries'!K20</f>
+        <v>2E-3</v>
+      </c>
+      <c r="C93" s="433">
+        <f>'Data Summaries'!K21</f>
+        <v>2E-3</v>
+      </c>
+      <c r="D93" s="433">
+        <f>'Data Summaries'!K22</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E93" s="433">
+        <f>'Data Summaries'!K23</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F93" s="433">
+        <f>'Data Summaries'!K24</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>681</v>
+      </c>
+      <c r="B94" s="433">
+        <f>'Data Summaries'!L20</f>
+        <v>0</v>
+      </c>
+      <c r="C94" s="433">
+        <f>'Data Summaries'!L21</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D94" s="433">
+        <f>'Data Summaries'!L22</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E94" s="433">
+        <f>'Data Summaries'!L23</f>
+        <v>0.01</v>
+      </c>
+      <c r="F94" s="433">
+        <f>'Data Summaries'!L24</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>682</v>
+      </c>
+      <c r="B95" s="433">
+        <f>'Data Summaries'!N20</f>
+        <v>0</v>
+      </c>
+      <c r="C95" s="433">
+        <f>'Data Summaries'!N21</f>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D95" s="433">
+        <f>'Data Summaries'!N22</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E95" s="433">
+        <f>'Data Summaries'!N23</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F95" s="433">
+        <f>'Data Summaries'!N24</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>683</v>
+      </c>
+      <c r="B96" s="433">
+        <f>'Data Summaries'!M20</f>
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="C96" s="433">
+        <f>'Data Summaries'!M21</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="D96" s="433">
+        <f>'Data Summaries'!M22</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E96" s="433">
+        <f>'Data Summaries'!M23</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F96" s="433">
+        <f>'Data Summaries'!M24</f>
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>685</v>
+      </c>
+      <c r="B97" s="26">
+        <f>'Data Summaries'!M64</f>
+        <v>8439</v>
+      </c>
+      <c r="C97" s="26">
+        <f>'Data Summaries'!M65</f>
+        <v>10529</v>
+      </c>
+      <c r="D97" s="26">
+        <f>'Data Summaries'!M66</f>
+        <v>6767</v>
+      </c>
+      <c r="E97" s="26">
+        <f>'Data Summaries'!M67</f>
+        <v>3118</v>
+      </c>
+      <c r="F97" s="26">
+        <f>'Data Summaries'!M68</f>
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>686</v>
+      </c>
+      <c r="B98" s="26">
+        <f>'Data Summaries'!X64</f>
+        <v>4604</v>
+      </c>
+      <c r="C98" s="26">
+        <f>'Data Summaries'!X65</f>
+        <v>4055</v>
+      </c>
+      <c r="D98" s="26">
+        <f>'Data Summaries'!X66</f>
+        <v>2073</v>
+      </c>
+      <c r="E98" s="26">
+        <f>'Data Summaries'!X67</f>
+        <v>642</v>
+      </c>
+      <c r="F98" s="26">
+        <f>'Data Summaries'!X68</f>
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700DC135-295E-45A6-9D8A-ABA304F30F0E}">
   <dimension ref="A1:L108"/>
   <sheetViews>
@@ -14449,7 +16955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6205817-3C53-46FD-A1E7-ECB63C82D6F9}">
   <dimension ref="A1:IU63"/>
   <sheetViews>
@@ -16888,7 +19394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1805004C-4081-426D-BC01-F05BBF9CAE23}">
   <dimension ref="A1:M158"/>
   <sheetViews>
@@ -22457,7 +24963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A1605B-3639-4A5F-B875-D10E7BB4922A}">
   <dimension ref="A1:H45"/>
   <sheetViews>
@@ -23187,7 +25693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28EDC59-5AE6-484B-AF0C-93F19C29C298}">
   <dimension ref="A1:BB41"/>
   <sheetViews>
@@ -23261,71 +25767,71 @@
     </row>
     <row r="2" spans="1:54">
       <c r="A2" s="223"/>
-      <c r="B2" s="416" t="s">
+      <c r="B2" s="410" t="s">
         <v>288</v>
       </c>
-      <c r="C2" s="416"/>
-      <c r="D2" s="416"/>
-      <c r="E2" s="416"/>
-      <c r="F2" s="416"/>
-      <c r="G2" s="416"/>
-      <c r="H2" s="416"/>
-      <c r="I2" s="416"/>
+      <c r="C2" s="410"/>
+      <c r="D2" s="410"/>
+      <c r="E2" s="410"/>
+      <c r="F2" s="410"/>
+      <c r="G2" s="410"/>
+      <c r="H2" s="410"/>
+      <c r="I2" s="410"/>
       <c r="J2" s="224"/>
-      <c r="K2" s="416" t="s">
+      <c r="K2" s="410" t="s">
         <v>289</v>
       </c>
-      <c r="L2" s="416"/>
-      <c r="M2" s="416"/>
-      <c r="N2" s="416"/>
-      <c r="O2" s="416"/>
-      <c r="P2" s="416"/>
-      <c r="Q2" s="416"/>
-      <c r="R2" s="416"/>
+      <c r="L2" s="410"/>
+      <c r="M2" s="410"/>
+      <c r="N2" s="410"/>
+      <c r="O2" s="410"/>
+      <c r="P2" s="410"/>
+      <c r="Q2" s="410"/>
+      <c r="R2" s="410"/>
       <c r="S2" s="224"/>
-      <c r="T2" s="416" t="s">
+      <c r="T2" s="410" t="s">
         <v>290</v>
       </c>
-      <c r="U2" s="416"/>
-      <c r="V2" s="416"/>
-      <c r="W2" s="416"/>
-      <c r="X2" s="416"/>
-      <c r="Y2" s="416"/>
-      <c r="Z2" s="416"/>
-      <c r="AA2" s="416"/>
+      <c r="U2" s="410"/>
+      <c r="V2" s="410"/>
+      <c r="W2" s="410"/>
+      <c r="X2" s="410"/>
+      <c r="Y2" s="410"/>
+      <c r="Z2" s="410"/>
+      <c r="AA2" s="410"/>
       <c r="AB2" s="224"/>
-      <c r="AC2" s="416" t="s">
+      <c r="AC2" s="410" t="s">
         <v>291</v>
       </c>
-      <c r="AD2" s="416"/>
-      <c r="AE2" s="416"/>
-      <c r="AF2" s="416"/>
-      <c r="AG2" s="416"/>
-      <c r="AH2" s="416"/>
-      <c r="AI2" s="416"/>
-      <c r="AJ2" s="416"/>
+      <c r="AD2" s="410"/>
+      <c r="AE2" s="410"/>
+      <c r="AF2" s="410"/>
+      <c r="AG2" s="410"/>
+      <c r="AH2" s="410"/>
+      <c r="AI2" s="410"/>
+      <c r="AJ2" s="410"/>
       <c r="AK2" s="224"/>
-      <c r="AL2" s="416" t="s">
+      <c r="AL2" s="410" t="s">
         <v>292</v>
       </c>
-      <c r="AM2" s="416"/>
-      <c r="AN2" s="416"/>
-      <c r="AO2" s="416"/>
-      <c r="AP2" s="416"/>
-      <c r="AQ2" s="416"/>
-      <c r="AR2" s="416"/>
-      <c r="AS2" s="416"/>
+      <c r="AM2" s="410"/>
+      <c r="AN2" s="410"/>
+      <c r="AO2" s="410"/>
+      <c r="AP2" s="410"/>
+      <c r="AQ2" s="410"/>
+      <c r="AR2" s="410"/>
+      <c r="AS2" s="410"/>
       <c r="AT2" s="225"/>
-      <c r="AU2" s="417" t="s">
+      <c r="AU2" s="411" t="s">
         <v>293</v>
       </c>
-      <c r="AV2" s="418"/>
-      <c r="AW2" s="418"/>
-      <c r="AX2" s="418"/>
-      <c r="AY2" s="418"/>
-      <c r="AZ2" s="418"/>
-      <c r="BA2" s="418"/>
-      <c r="BB2" s="418"/>
+      <c r="AV2" s="412"/>
+      <c r="AW2" s="412"/>
+      <c r="AX2" s="412"/>
+      <c r="AY2" s="412"/>
+      <c r="AZ2" s="412"/>
+      <c r="BA2" s="412"/>
+      <c r="BB2" s="412"/>
     </row>
     <row r="3" spans="1:54" ht="25.5" customHeight="1">
       <c r="A3" s="226"/>
@@ -23344,20 +25850,20 @@
       </c>
       <c r="I3" s="414"/>
       <c r="J3" s="228"/>
-      <c r="K3" s="419" t="s">
+      <c r="K3" s="413" t="s">
         <v>294</v>
       </c>
-      <c r="L3" s="419"/>
+      <c r="L3" s="413"/>
       <c r="M3" s="229"/>
-      <c r="N3" s="419" t="s">
+      <c r="N3" s="413" t="s">
         <v>295</v>
       </c>
-      <c r="O3" s="419"/>
+      <c r="O3" s="413"/>
       <c r="P3" s="229"/>
-      <c r="Q3" s="419" t="s">
+      <c r="Q3" s="413" t="s">
         <v>296</v>
       </c>
-      <c r="R3" s="419"/>
+      <c r="R3" s="413"/>
       <c r="S3" s="227"/>
       <c r="T3" s="414" t="s">
         <v>294</v>
@@ -24724,85 +27230,85 @@
     </row>
     <row r="22" spans="1:42">
       <c r="A22" s="264"/>
-      <c r="B22" s="410" t="s">
+      <c r="B22" s="417" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="410"/>
-      <c r="D22" s="410"/>
-      <c r="E22" s="410"/>
-      <c r="F22" s="410"/>
-      <c r="G22" s="410"/>
-      <c r="H22" s="410"/>
-      <c r="I22" s="410"/>
+      <c r="C22" s="417"/>
+      <c r="D22" s="417"/>
+      <c r="E22" s="417"/>
+      <c r="F22" s="417"/>
+      <c r="G22" s="417"/>
+      <c r="H22" s="417"/>
+      <c r="I22" s="417"/>
       <c r="J22" s="265"/>
-      <c r="K22" s="410" t="s">
+      <c r="K22" s="417" t="s">
         <v>181</v>
       </c>
-      <c r="L22" s="410"/>
-      <c r="M22" s="410"/>
-      <c r="N22" s="410"/>
-      <c r="O22" s="410"/>
-      <c r="P22" s="410"/>
-      <c r="Q22" s="410"/>
-      <c r="R22" s="410"/>
+      <c r="L22" s="417"/>
+      <c r="M22" s="417"/>
+      <c r="N22" s="417"/>
+      <c r="O22" s="417"/>
+      <c r="P22" s="417"/>
+      <c r="Q22" s="417"/>
+      <c r="R22" s="417"/>
       <c r="S22" s="265"/>
-      <c r="T22" s="410" t="s">
+      <c r="T22" s="417" t="s">
         <v>433</v>
       </c>
-      <c r="U22" s="410"/>
-      <c r="V22" s="410"/>
-      <c r="W22" s="410"/>
-      <c r="X22" s="410"/>
-      <c r="Y22" s="410"/>
-      <c r="Z22" s="410"/>
-      <c r="AA22" s="410"/>
+      <c r="U22" s="417"/>
+      <c r="V22" s="417"/>
+      <c r="W22" s="417"/>
+      <c r="X22" s="417"/>
+      <c r="Y22" s="417"/>
+      <c r="Z22" s="417"/>
+      <c r="AA22" s="417"/>
     </row>
     <row r="23" spans="1:42" ht="22.5" customHeight="1">
       <c r="A23" s="266"/>
-      <c r="B23" s="411" t="s">
+      <c r="B23" s="418" t="s">
         <v>294</v>
       </c>
-      <c r="C23" s="411"/>
+      <c r="C23" s="418"/>
       <c r="D23" s="267"/>
-      <c r="E23" s="412" t="s">
+      <c r="E23" s="416" t="s">
         <v>295</v>
       </c>
-      <c r="F23" s="412"/>
+      <c r="F23" s="416"/>
       <c r="G23" s="268"/>
-      <c r="H23" s="413" t="s">
+      <c r="H23" s="419" t="s">
         <v>296</v>
       </c>
-      <c r="I23" s="413"/>
+      <c r="I23" s="419"/>
       <c r="J23" s="269"/>
-      <c r="K23" s="411" t="s">
+      <c r="K23" s="418" t="s">
         <v>294</v>
       </c>
-      <c r="L23" s="411"/>
+      <c r="L23" s="418"/>
       <c r="M23" s="267"/>
-      <c r="N23" s="412" t="s">
+      <c r="N23" s="416" t="s">
         <v>295</v>
       </c>
-      <c r="O23" s="412"/>
+      <c r="O23" s="416"/>
       <c r="P23" s="268"/>
-      <c r="Q23" s="413" t="s">
+      <c r="Q23" s="419" t="s">
         <v>296</v>
       </c>
-      <c r="R23" s="413"/>
+      <c r="R23" s="419"/>
       <c r="S23" s="269"/>
-      <c r="T23" s="412" t="s">
+      <c r="T23" s="416" t="s">
         <v>294</v>
       </c>
-      <c r="U23" s="412"/>
+      <c r="U23" s="416"/>
       <c r="V23" s="268"/>
-      <c r="W23" s="412" t="s">
+      <c r="W23" s="416" t="s">
         <v>295</v>
       </c>
-      <c r="X23" s="412"/>
+      <c r="X23" s="416"/>
       <c r="Y23" s="270"/>
-      <c r="Z23" s="412" t="s">
+      <c r="Z23" s="416" t="s">
         <v>296</v>
       </c>
-      <c r="AA23" s="412"/>
+      <c r="AA23" s="416"/>
     </row>
     <row r="24" spans="1:42">
       <c r="A24" s="271" t="s">
@@ -25641,6 +28147,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="T22:AA22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AX3:AY3"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AO3:AP3"/>
     <mergeCell ref="AL2:AS2"/>
     <mergeCell ref="AU2:BB2"/>
     <mergeCell ref="Q3:R3"/>
@@ -25657,37 +28183,17 @@
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="W3:X3"/>
     <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AX3:AY3"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="T22:AA22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="T23:U23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B37301-E1FE-4294-8D48-65F6FF26C74D}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26059,11 +28565,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2383582F-E559-4175-AFC0-39080E0B28DD}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
@@ -26074,11 +28580,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="43.5" customHeight="1">
-      <c r="A1" s="431" t="s">
+      <c r="A1" s="428" t="s">
         <v>561</v>
       </c>
-      <c r="B1" s="431"/>
-      <c r="C1" s="431"/>
+      <c r="B1" s="428"/>
+      <c r="C1" s="428"/>
       <c r="D1" s="318"/>
       <c r="E1" s="318"/>
       <c r="F1" s="318"/>
@@ -26245,11 +28751,11 @@
       <c r="H18" s="331"/>
     </row>
     <row r="19" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A19" s="427" t="s">
+      <c r="A19" s="429" t="s">
         <v>575</v>
       </c>
-      <c r="B19" s="427"/>
-      <c r="C19" s="427"/>
+      <c r="B19" s="429"/>
+      <c r="C19" s="429"/>
       <c r="D19" s="331"/>
       <c r="E19" s="331"/>
       <c r="F19" s="331"/>
@@ -26257,11 +28763,11 @@
       <c r="H19" s="331"/>
     </row>
     <row r="20" spans="1:15" ht="46.5" customHeight="1">
-      <c r="A20" s="427" t="s">
+      <c r="A20" s="429" t="s">
         <v>576</v>
       </c>
-      <c r="B20" s="427"/>
-      <c r="C20" s="427"/>
+      <c r="B20" s="429"/>
+      <c r="C20" s="429"/>
       <c r="D20" s="331"/>
       <c r="E20" s="331"/>
       <c r="F20" s="331"/>
@@ -26269,11 +28775,11 @@
       <c r="H20" s="331"/>
     </row>
     <row r="21" spans="1:15" ht="59.25" customHeight="1">
-      <c r="A21" s="427" t="s">
+      <c r="A21" s="429" t="s">
         <v>577</v>
       </c>
-      <c r="B21" s="427"/>
-      <c r="C21" s="427"/>
+      <c r="B21" s="429"/>
+      <c r="C21" s="429"/>
       <c r="D21" s="333"/>
       <c r="E21" s="333"/>
       <c r="F21" s="333"/>
@@ -26281,11 +28787,11 @@
       <c r="H21" s="333"/>
     </row>
     <row r="22" spans="1:15" ht="26.25" customHeight="1">
-      <c r="A22" s="427" t="s">
+      <c r="A22" s="429" t="s">
         <v>429</v>
       </c>
-      <c r="B22" s="427"/>
-      <c r="C22" s="427"/>
+      <c r="B22" s="429"/>
+      <c r="C22" s="429"/>
       <c r="D22" s="334"/>
       <c r="E22" s="335"/>
       <c r="F22" s="335"/>
@@ -26323,15 +28829,15 @@
       <c r="C25" s="336"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="430" t="s">
+      <c r="A26" s="427" t="s">
         <v>579</v>
       </c>
-      <c r="B26" s="430"/>
-      <c r="C26" s="430"/>
-      <c r="D26" s="430"/>
-      <c r="E26" s="430"/>
-      <c r="F26" s="430"/>
-      <c r="G26" s="430"/>
+      <c r="B26" s="427"/>
+      <c r="C26" s="427"/>
+      <c r="D26" s="427"/>
+      <c r="E26" s="427"/>
+      <c r="F26" s="427"/>
+      <c r="G26" s="427"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="338"/>
@@ -26344,29 +28850,29 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="340"/>
-      <c r="B28" s="428" t="s">
+      <c r="B28" s="430" t="s">
         <v>580</v>
       </c>
-      <c r="C28" s="428"/>
-      <c r="D28" s="428"/>
-      <c r="E28" s="428"/>
-      <c r="F28" s="428"/>
-      <c r="G28" s="428"/>
+      <c r="C28" s="430"/>
+      <c r="D28" s="430"/>
+      <c r="E28" s="430"/>
+      <c r="F28" s="430"/>
+      <c r="G28" s="430"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="341"/>
-      <c r="B29" s="429" t="s">
+      <c r="B29" s="431" t="s">
         <v>180</v>
       </c>
-      <c r="C29" s="429"/>
-      <c r="D29" s="429" t="s">
+      <c r="C29" s="431"/>
+      <c r="D29" s="431" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="429"/>
-      <c r="F29" s="429" t="s">
+      <c r="E29" s="431"/>
+      <c r="F29" s="431" t="s">
         <v>433</v>
       </c>
-      <c r="G29" s="429"/>
+      <c r="G29" s="431"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="342" t="s">
@@ -26587,48 +29093,48 @@
       <c r="G39" s="339"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="427" t="s">
+      <c r="A40" s="429" t="s">
         <v>604</v>
       </c>
-      <c r="B40" s="427"/>
-      <c r="C40" s="427"/>
-      <c r="D40" s="427"/>
-      <c r="E40" s="427"/>
-      <c r="F40" s="427"/>
-      <c r="G40" s="427"/>
+      <c r="B40" s="429"/>
+      <c r="C40" s="429"/>
+      <c r="D40" s="429"/>
+      <c r="E40" s="429"/>
+      <c r="F40" s="429"/>
+      <c r="G40" s="429"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="427" t="s">
+      <c r="A41" s="429" t="s">
         <v>577</v>
       </c>
-      <c r="B41" s="427"/>
-      <c r="C41" s="427"/>
-      <c r="D41" s="427"/>
-      <c r="E41" s="427"/>
-      <c r="F41" s="427"/>
-      <c r="G41" s="427"/>
+      <c r="B41" s="429"/>
+      <c r="C41" s="429"/>
+      <c r="D41" s="429"/>
+      <c r="E41" s="429"/>
+      <c r="F41" s="429"/>
+      <c r="G41" s="429"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="427" t="s">
+      <c r="A42" s="429" t="s">
         <v>429</v>
       </c>
-      <c r="B42" s="427"/>
-      <c r="C42" s="427"/>
-      <c r="D42" s="427"/>
-      <c r="E42" s="427"/>
-      <c r="F42" s="427"/>
-      <c r="G42" s="427"/>
+      <c r="B42" s="429"/>
+      <c r="C42" s="429"/>
+      <c r="D42" s="429"/>
+      <c r="E42" s="429"/>
+      <c r="F42" s="429"/>
+      <c r="G42" s="429"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="427" t="s">
+      <c r="A43" s="429" t="s">
         <v>605</v>
       </c>
-      <c r="B43" s="427"/>
-      <c r="C43" s="427"/>
-      <c r="D43" s="427"/>
-      <c r="E43" s="427"/>
-      <c r="F43" s="427"/>
-      <c r="G43" s="427"/>
+      <c r="B43" s="429"/>
+      <c r="C43" s="429"/>
+      <c r="D43" s="429"/>
+      <c r="E43" s="429"/>
+      <c r="F43" s="429"/>
+      <c r="G43" s="429"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="339"/>
@@ -26652,12 +29158,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="A43:G43"/>
     <mergeCell ref="B28:G28"/>
@@ -26666,6 +29166,12 @@
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="A40:G40"/>
     <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>